<commit_message>
fixed armors text loading
</commit_message>
<xml_diff>
--- a/doc/items.xlsx
+++ b/doc/items.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="Ten_skoroszyt" defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomasz.zielski\Source\Repos\carpg\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr codeName="Ten_skoroszyt"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="armor" sheetId="1" r:id="rId1"/>
     <sheet name="weapon" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -402,8 +397,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -506,7 +501,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -517,6 +511,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -577,7 +573,7 @@
     </a:clrScheme>
     <a:fontScheme name="Pakiet Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -612,7 +608,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -789,54 +785,54 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Arkusz1"/>
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="11"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11" t="s">
+      <c r="H1" s="10"/>
+      <c r="I1" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -861,7 +857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -886,7 +882,7 @@
         <v>7.8571428571428568</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>44</v>
@@ -911,7 +907,7 @@
         <v>33.666666666666664</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>5</v>
@@ -936,7 +932,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>6</v>
@@ -961,7 +957,7 @@
         <v>5.416666666666667</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>7</v>
@@ -986,7 +982,7 @@
         <v>25.75</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>8</v>
@@ -1011,7 +1007,7 @@
         <v>127.54545454545455</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>9</v>
@@ -1036,7 +1032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
         <v>10</v>
@@ -1061,7 +1057,7 @@
         <v>4.4444444444444446</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>11</v>
@@ -1086,7 +1082,7 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -1111,7 +1107,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>13</v>
@@ -1136,7 +1132,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>14</v>
@@ -1161,7 +1157,7 @@
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
         <v>45</v>
@@ -1185,12 +1181,12 @@
         <f t="shared" si="2"/>
         <v>31.428571428571427</v>
       </c>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
         <v>15</v>
@@ -1214,12 +1210,12 @@
         <f t="shared" si="2"/>
         <v>74.285714285714292</v>
       </c>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>16</v>
@@ -1243,12 +1239,12 @@
         <f t="shared" si="2"/>
         <v>250</v>
       </c>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="6"/>
       <c r="B18" s="7" t="s">
         <v>17</v>
@@ -1274,7 +1270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
         <v>18</v>
@@ -1299,7 +1295,7 @@
         <v>3.6111111111111112</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
         <v>46</v>
@@ -1324,7 +1320,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
@@ -1349,7 +1345,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -1374,7 +1370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
         <v>21</v>
@@ -1399,7 +1395,7 @@
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" s="4"/>
       <c r="B24" t="s">
         <v>47</v>
@@ -1424,7 +1420,7 @@
         <v>35.333333333333336</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" s="4"/>
       <c r="B25" s="2" t="s">
         <v>22</v>
@@ -1449,7 +1445,7 @@
         <v>68.666666666666671</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" s="4"/>
       <c r="B26" s="2" t="s">
         <v>23</v>
@@ -1474,7 +1470,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" s="4"/>
       <c r="B27" s="2" t="s">
         <v>24</v>
@@ -1499,7 +1495,7 @@
         <v>8.6206896551724146</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" s="4"/>
       <c r="B28" s="2" t="s">
         <v>25</v>
@@ -1524,12 +1520,12 @@
         <f t="shared" si="2"/>
         <v>32.857142857142854</v>
       </c>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="4"/>
       <c r="B29" s="2" t="s">
         <v>26</v>
@@ -1554,12 +1550,12 @@
         <f t="shared" si="2"/>
         <v>135.83333333333334</v>
       </c>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="4"/>
       <c r="B30" t="s">
         <v>27</v>
@@ -1583,12 +1579,12 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="4"/>
       <c r="B31" t="s">
         <v>28</v>
@@ -1612,12 +1608,12 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="4"/>
       <c r="B32" s="5" t="s">
         <v>49</v>
@@ -1641,12 +1637,12 @@
         <f t="shared" si="2"/>
         <v>31.75</v>
       </c>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="4"/>
       <c r="B33" s="2" t="s">
         <v>48</v>
@@ -1671,7 +1667,7 @@
         <v>81.75</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9">
       <c r="A34" s="4"/>
       <c r="B34" s="2" t="s">
         <v>29</v>
@@ -1696,258 +1692,260 @@
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="2" t="s">
+    <row r="35" spans="1:9">
+      <c r="A35" s="16"/>
+      <c r="B35" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="14">
         <v>135</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="14">
         <v>22000</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="14">
         <v>80</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="14">
         <v>45</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="14">
         <v>65</v>
       </c>
-      <c r="I35">
+      <c r="H35" s="15"/>
+      <c r="I35" s="15">
         <f t="shared" si="3"/>
         <v>275</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="7">
-        <v>180</v>
-      </c>
-      <c r="D36" s="7">
-        <v>100</v>
-      </c>
-      <c r="E36" s="7">
-        <v>25</v>
-      </c>
-      <c r="F36" s="7">
-        <v>50</v>
-      </c>
-      <c r="G36" s="7">
-        <v>45</v>
-      </c>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9">
+      <c r="A36" s="3"/>
+      <c r="B36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="2">
+        <v>225</v>
+      </c>
+      <c r="D36" s="2">
+        <v>350</v>
+      </c>
+      <c r="E36" s="2">
+        <v>35</v>
+      </c>
+      <c r="F36" s="2">
+        <v>60</v>
+      </c>
+      <c r="G36" s="2">
+        <v>40</v>
+      </c>
+      <c r="I36">
+        <f>IFERROR(D36/E36,"---")</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="3"/>
       <c r="B37" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C37" s="2">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="D37" s="2">
-        <v>300</v>
+        <v>650</v>
       </c>
       <c r="E37" s="2">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F37" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G37" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I37">
-        <f t="shared" si="3"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <f>IFERROR(D37/E37,"---")</f>
+        <v>16.25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="2">
+        <v>200</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1350</v>
+      </c>
+      <c r="E38" s="2">
+        <v>45</v>
+      </c>
+      <c r="F38" s="2">
+        <v>55</v>
+      </c>
+      <c r="G38" s="2">
+        <v>45</v>
+      </c>
+      <c r="I38">
+        <f>IFERROR(D38/E38,"---")</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="19"/>
+      <c r="B39" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="20">
+        <v>115</v>
+      </c>
+      <c r="D39" s="20">
+        <v>2950</v>
+      </c>
+      <c r="E39" s="20">
+        <v>45</v>
+      </c>
+      <c r="F39" s="20">
+        <v>40</v>
+      </c>
+      <c r="G39" s="20">
+        <v>60</v>
+      </c>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9">
+        <f>IFERROR(D39/E39,"---")</f>
+        <v>65.555555555555557</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="19"/>
+      <c r="B40" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="20">
+        <v>180</v>
+      </c>
+      <c r="D40" s="20">
+        <v>100</v>
+      </c>
+      <c r="E40" s="20">
+        <v>25</v>
+      </c>
+      <c r="F40" s="20">
         <v>50</v>
       </c>
-      <c r="C38" s="2">
-        <v>160</v>
-      </c>
-      <c r="D38" s="2">
-        <v>1100</v>
-      </c>
-      <c r="E38" s="2">
-        <v>35</v>
-      </c>
-      <c r="F38" s="2">
-        <v>50</v>
-      </c>
-      <c r="G38" s="2">
-        <v>50</v>
-      </c>
-      <c r="I38">
-        <f t="shared" ref="I38" si="4">IFERROR(D38/E38,"---")</f>
-        <v>31.428571428571427</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="2">
-        <v>90</v>
-      </c>
-      <c r="D39" s="2">
-        <v>3100</v>
-      </c>
-      <c r="E39" s="2">
-        <v>35</v>
-      </c>
-      <c r="F39" s="2">
-        <v>35</v>
-      </c>
-      <c r="G39" s="2">
-        <v>65</v>
-      </c>
-      <c r="I39">
-        <f t="shared" ref="I39" si="5">IFERROR(D39/E39,"---")</f>
-        <v>88.571428571428569</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C40" s="2">
-        <v>200</v>
-      </c>
-      <c r="D40" s="2">
-        <v>18000</v>
-      </c>
-      <c r="E40" s="2">
-        <v>65</v>
-      </c>
-      <c r="F40" s="2">
-        <v>55</v>
-      </c>
-      <c r="G40" s="2">
-        <v>50</v>
-      </c>
-      <c r="I40">
-        <f t="shared" ref="I40:I52" si="6">IFERROR(D40/E40,"---")</f>
-        <v>276.92307692307691</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G40" s="20">
+        <v>45</v>
+      </c>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9">
+        <f>IFERROR(D40/E40,"---")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="3"/>
       <c r="B41" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C41" s="2">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D41" s="2">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="E41" s="2">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F41" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G41" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I41">
-        <f t="shared" si="6"/>
+        <f>IFERROR(D41/E41,"---")</f>
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9">
       <c r="A42" s="3"/>
       <c r="B42" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="2">
+        <v>160</v>
+      </c>
+      <c r="D42" s="2">
+        <v>1100</v>
+      </c>
+      <c r="E42" s="2">
         <v>35</v>
       </c>
-      <c r="C42" s="2">
-        <v>225</v>
-      </c>
-      <c r="D42" s="2">
-        <v>650</v>
-      </c>
-      <c r="E42" s="2">
-        <v>40</v>
-      </c>
       <c r="F42" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G42" s="2">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="I42">
-        <f t="shared" si="6"/>
-        <v>16.25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I42" si="4">IFERROR(D42/E42,"---")</f>
+        <v>31.428571428571427</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="3"/>
       <c r="B43" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="2">
-        <v>200</v>
+        <v>90</v>
       </c>
       <c r="D43" s="2">
-        <v>1350</v>
+        <v>3100</v>
       </c>
       <c r="E43" s="2">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="F43" s="2">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="G43" s="2">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="I43">
-        <f t="shared" si="6"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I43" si="5">IFERROR(D43/E43,"---")</f>
+        <v>88.571428571428569</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="3"/>
       <c r="B44" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C44" s="2">
-        <v>115</v>
+        <v>200</v>
       </c>
       <c r="D44" s="2">
-        <v>2950</v>
+        <v>18000</v>
       </c>
       <c r="E44" s="2">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="F44" s="2">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="G44" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="I44">
-        <f t="shared" si="6"/>
-        <v>65.555555555555557</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+        <f>IFERROR(D44/E44,"---")</f>
+        <v>276.92307692307691</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="3"/>
       <c r="B45" t="s">
         <v>37</v>
@@ -1968,11 +1966,11 @@
         <v>30</v>
       </c>
       <c r="I45">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="I40:I52" si="6">IFERROR(D45/E45,"---")</f>
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9">
       <c r="A46" s="3"/>
       <c r="B46" t="s">
         <v>38</v>
@@ -1997,7 +1995,7 @@
         <v>30.90909090909091</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9">
       <c r="A47" s="3"/>
       <c r="B47" t="s">
         <v>39</v>
@@ -2023,7 +2021,7 @@
         <v>58.333333333333336</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" s="3"/>
       <c r="B48" s="2" t="s">
         <v>53</v>
@@ -2048,7 +2046,7 @@
         <v>116.66666666666667</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" s="3"/>
       <c r="B49" t="s">
         <v>40</v>
@@ -2073,7 +2071,7 @@
         <v>131.25</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" s="3"/>
       <c r="B50" t="s">
         <v>41</v>
@@ -2098,7 +2096,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" s="3"/>
       <c r="B51" t="s">
         <v>42</v>
@@ -2123,7 +2121,7 @@
         <v>92.307692307692307</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" s="3"/>
       <c r="B52" s="2" t="s">
         <v>43</v>
@@ -2150,11 +2148,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2:I52">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -2167,40 +2165,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:7">
+      <c r="B1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>59</v>
@@ -2222,7 +2220,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>61</v>
@@ -2235,7 +2233,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>62</v>
@@ -2248,7 +2246,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>67</v>
@@ -2270,7 +2268,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>63</v>
@@ -2292,7 +2290,7 @@
         <v>312.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>60</v>
@@ -2314,7 +2312,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>65</v>
@@ -2327,7 +2325,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>66</v>
@@ -2340,7 +2338,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
         <v>64</v>
@@ -2362,7 +2360,7 @@
         <v>83.333333333333329</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>68</v>
@@ -2384,7 +2382,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>69</v>
@@ -2397,7 +2395,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>70</v>
@@ -2410,23 +2408,23 @@
         <v>---</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="15" t="s">
+    <row r="14" spans="1:7">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="14">
         <v>10</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>---</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
         <v>71</v>
@@ -2448,7 +2446,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
         <v>72</v>
@@ -2461,7 +2459,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>73</v>
@@ -2474,7 +2472,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
         <v>74</v>
@@ -2496,7 +2494,7 @@
         <v>21.818181818181817</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
         <v>75</v>
@@ -2518,7 +2516,7 @@
         <v>133.33333333333334</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
         <v>77</v>
@@ -2534,7 +2532,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>76</v>
@@ -2556,7 +2554,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
         <v>79</v>
@@ -2569,7 +2567,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
         <v>80</v>
@@ -2582,7 +2580,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="4"/>
       <c r="B24" s="2" t="s">
         <v>81</v>
@@ -2599,7 +2597,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="4"/>
       <c r="B25" t="s">
         <v>82</v>
@@ -2621,22 +2619,22 @@
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
-      <c r="B26" s="16" t="s">
+    <row r="26" spans="1:7">
+      <c r="A26" s="16"/>
+      <c r="B26" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="16">
+      <c r="C26" s="15">
         <f>18*1.5</f>
         <v>27</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="15">
         <v>25</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="15">
         <v>40</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="15">
         <v>55</v>
       </c>
       <c r="G26">
@@ -2644,7 +2642,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="3"/>
       <c r="B27" t="s">
         <v>84</v>
@@ -2666,7 +2664,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="3"/>
       <c r="B28" t="s">
         <v>85</v>
@@ -2679,7 +2677,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="3"/>
       <c r="B29" t="s">
         <v>86</v>
@@ -2692,7 +2690,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
         <v>87</v>
@@ -2709,7 +2707,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="3"/>
       <c r="B31" t="s">
         <v>88</v>
@@ -2731,7 +2729,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="3"/>
       <c r="B32" t="s">
         <v>89</v>
@@ -2744,7 +2742,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="3"/>
       <c r="B33" t="s">
         <v>90</v>
@@ -2757,7 +2755,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="3"/>
       <c r="B34" t="s">
         <v>91</v>
@@ -2779,7 +2777,7 @@
         <v>94.117647058823536</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="3"/>
       <c r="B35" s="2" t="s">
         <v>92</v>
@@ -2795,7 +2793,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="3"/>
       <c r="B36" t="s">
         <v>93</v>
@@ -2817,7 +2815,7 @@
         <v>36.363636363636367</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="3"/>
       <c r="B37" s="2" t="s">
         <v>94</v>
@@ -2833,7 +2831,7 @@
         <v>---</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="3"/>
       <c r="B38" t="s">
         <v>95</v>
@@ -2855,21 +2853,21 @@
         <v>363.63636363636363</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="16" t="s">
+    <row r="39" spans="1:7">
+      <c r="A39" s="17"/>
+      <c r="B39" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C39" s="16">
+      <c r="C39" s="15">
         <v>36</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="15">
         <v>25</v>
       </c>
-      <c r="E39" s="16">
+      <c r="E39" s="15">
         <v>35</v>
       </c>
-      <c r="F39" s="16">
+      <c r="F39" s="15">
         <v>75</v>
       </c>
       <c r="G39">
@@ -2877,8 +2875,8 @@
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
+    <row r="40" spans="1:7">
+      <c r="A40" s="11"/>
       <c r="B40" t="s">
         <v>97</v>
       </c>
@@ -2899,8 +2897,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
+    <row r="41" spans="1:7">
+      <c r="A41" s="11"/>
       <c r="B41" t="s">
         <v>98</v>
       </c>
@@ -2912,8 +2910,8 @@
         <v>---</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
+    <row r="42" spans="1:7">
+      <c r="A42" s="11"/>
       <c r="B42" t="s">
         <v>99</v>
       </c>
@@ -2925,8 +2923,8 @@
         <v>---</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
+    <row r="43" spans="1:7">
+      <c r="A43" s="11"/>
       <c r="B43" t="s">
         <v>101</v>
       </c>
@@ -2947,8 +2945,8 @@
         <v>0.34285714285714286</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
+    <row r="44" spans="1:7">
+      <c r="A44" s="11"/>
       <c r="B44" t="s">
         <v>102</v>
       </c>
@@ -2960,8 +2958,8 @@
         <v>---</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
+    <row r="45" spans="1:7">
+      <c r="A45" s="11"/>
       <c r="B45" t="s">
         <v>103</v>
       </c>
@@ -2973,8 +2971,8 @@
         <v>---</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
+    <row r="46" spans="1:7">
+      <c r="A46" s="11"/>
       <c r="B46" t="s">
         <v>104</v>
       </c>
@@ -2995,8 +2993,8 @@
         <v>55.555555555555557</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
+    <row r="47" spans="1:7">
+      <c r="A47" s="11"/>
       <c r="B47" s="2" t="s">
         <v>100</v>
       </c>
@@ -3017,8 +3015,8 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
+    <row r="48" spans="1:7">
+      <c r="A48" s="11"/>
       <c r="B48" s="2" t="s">
         <v>105</v>
       </c>
@@ -3033,8 +3031,8 @@
         <v>---</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
+    <row r="49" spans="1:7">
+      <c r="A49" s="11"/>
       <c r="B49" s="2" t="s">
         <v>106</v>
       </c>
@@ -3050,8 +3048,8 @@
         <v>---</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="12"/>
+    <row r="50" spans="1:7">
+      <c r="A50" s="11"/>
       <c r="B50" t="s">
         <v>107</v>
       </c>
@@ -3072,8 +3070,8 @@
         <v>8.3333333333333339</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="12"/>
+    <row r="51" spans="1:7">
+      <c r="A51" s="11"/>
       <c r="B51" s="2" t="s">
         <v>108</v>
       </c>
@@ -3089,8 +3087,8 @@
         <v>---</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="12"/>
+    <row r="52" spans="1:7">
+      <c r="A52" s="11"/>
       <c r="B52" s="2" t="s">
         <v>114</v>
       </c>
@@ -3105,8 +3103,8 @@
         <v>---</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
+    <row r="53" spans="1:7">
+      <c r="A53" s="11"/>
       <c r="B53" t="s">
         <v>109</v>
       </c>
@@ -3124,8 +3122,8 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
+    <row r="54" spans="1:7">
+      <c r="A54" s="11"/>
       <c r="B54" t="s">
         <v>110</v>
       </c>
@@ -3137,8 +3135,8 @@
         <v>---</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
+    <row r="55" spans="1:7">
+      <c r="A55" s="11"/>
       <c r="B55" t="s">
         <v>111</v>
       </c>
@@ -3150,8 +3148,8 @@
         <v>---</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
+    <row r="56" spans="1:7">
+      <c r="A56" s="11"/>
       <c r="B56" s="2" t="s">
         <v>112</v>
       </c>
@@ -3166,8 +3164,8 @@
         <v>---</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
+    <row r="57" spans="1:7">
+      <c r="A57" s="11"/>
       <c r="B57" t="s">
         <v>113</v>
       </c>
@@ -3188,8 +3186,8 @@
         <v>208.33333333333334</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
+    <row r="58" spans="1:7">
+      <c r="A58" s="11"/>
       <c r="B58" t="s">
         <v>115</v>
       </c>
@@ -3210,8 +3208,8 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="12"/>
+    <row r="59" spans="1:7">
+      <c r="A59" s="11"/>
       <c r="B59" t="s">
         <v>122</v>
       </c>
@@ -3232,8 +3230,8 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
+    <row r="60" spans="1:7">
+      <c r="A60" s="11"/>
       <c r="B60" t="s">
         <v>116</v>
       </c>
@@ -3254,24 +3252,24 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
-      <c r="B61" s="16" t="s">
+    <row r="61" spans="1:7">
+      <c r="A61" s="18"/>
+      <c r="B61" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="C61" s="16">
+      <c r="C61" s="15">
         <v>30</v>
       </c>
-      <c r="D61" s="16"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
         <v>---</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
+    <row r="62" spans="1:7">
+      <c r="A62" s="12"/>
       <c r="B62" t="s">
         <v>118</v>
       </c>
@@ -3292,8 +3290,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
+    <row r="63" spans="1:7">
+      <c r="A63" s="12"/>
       <c r="B63" t="s">
         <v>119</v>
       </c>
@@ -3314,8 +3312,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
+    <row r="64" spans="1:7">
+      <c r="A64" s="12"/>
       <c r="B64" t="s">
         <v>120</v>
       </c>
@@ -3336,8 +3334,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
+    <row r="65" spans="1:7">
+      <c r="A65" s="12"/>
       <c r="B65" t="s">
         <v>121</v>
       </c>
@@ -3362,9 +3360,9 @@
   <conditionalFormatting sqref="G2:G65">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>

</xml_diff>

<commit_message>
armors desc, effects example, armor ids changes
</commit_message>
<xml_diff>
--- a/doc/items.xlsx
+++ b/doc/items.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="Ten_skoroszyt"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomasz.zielski\Source\Repos\carpg\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="armor" sheetId="1" r:id="rId1"/>
     <sheet name="weapon" sheetId="2" r:id="rId2"/>
+    <sheet name="shield" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="166">
   <si>
     <t>def</t>
   </si>
@@ -181,9 +187,6 @@
     <t>plated m</t>
   </si>
   <si>
-    <t>plate mih</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -392,13 +395,142 @@
   </si>
   <si>
     <t>value/dmg</t>
+  </si>
+  <si>
+    <t>10 magic res</t>
+  </si>
+  <si>
+    <t>1% hp reg aura, 25 negative res, 25 magic res</t>
+  </si>
+  <si>
+    <t>+15 dex, +15 thief skills, 20 magic res</t>
+  </si>
+  <si>
+    <t>25 fires res, 10 magic res</t>
+  </si>
+  <si>
+    <t>+10 str, +10 con, 2% reg</t>
+  </si>
+  <si>
+    <t>10 mres</t>
+  </si>
+  <si>
+    <t>25 fire res, 10 magic res</t>
+  </si>
+  <si>
+    <t>15 magic res</t>
+  </si>
+  <si>
+    <t>25 magic res, +10 str/dex/con, +10 weapon skills, +10 medium armor</t>
+  </si>
+  <si>
+    <t>plate mith</t>
+  </si>
+  <si>
+    <t>15 mres</t>
+  </si>
+  <si>
+    <t>25 mres, +15 str/con, 15% damage purge around (negative)</t>
+  </si>
+  <si>
+    <t>crystal m</t>
+  </si>
+  <si>
+    <t>20 mres, +5% lifesteal, +5% str to dmg (max 30(40 for decrasing), decrase 1/sec), glow when full</t>
+  </si>
+  <si>
+    <t>50 mres, 10% mana burn</t>
+  </si>
+  <si>
+    <t>wood hq</t>
+  </si>
+  <si>
+    <t>wood</t>
+  </si>
+  <si>
+    <t>wood m</t>
+  </si>
+  <si>
+    <t>elfwood (hq)</t>
+  </si>
+  <si>
+    <t>elfwood m</t>
+  </si>
+  <si>
+    <t>iron</t>
+  </si>
+  <si>
+    <t>iron hq</t>
+  </si>
+  <si>
+    <t>iron m</t>
+  </si>
+  <si>
+    <t>mith</t>
+  </si>
+  <si>
+    <t>adam</t>
+  </si>
+  <si>
+    <t>the wall</t>
+  </si>
+  <si>
+    <t>buckler</t>
+  </si>
+  <si>
+    <t>buckler hq</t>
+  </si>
+  <si>
+    <t>buckler m</t>
+  </si>
+  <si>
+    <t>tower</t>
+  </si>
+  <si>
+    <t>tower hq</t>
+  </si>
+  <si>
+    <t>tower m</t>
+  </si>
+  <si>
+    <t>spiky shield (hq)</t>
+  </si>
+  <si>
+    <t>spiky shield m</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>energy shield</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>info</t>
+  </si>
+  <si>
+    <t>price/def</t>
+  </si>
+  <si>
+    <t>mres 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,6 +547,13 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF0000FF"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="8">
@@ -491,7 +630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -513,6 +652,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -785,38 +927,39 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Arkusz1"/>
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="2.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>0</v>
@@ -829,10 +972,10 @@
       </c>
       <c r="H1" s="10"/>
       <c r="I1" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -857,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -882,7 +1025,7 @@
         <v>7.8571428571428568</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>44</v>
@@ -907,7 +1050,7 @@
         <v>33.666666666666664</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>5</v>
@@ -932,7 +1075,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>6</v>
@@ -957,7 +1100,7 @@
         <v>5.416666666666667</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>7</v>
@@ -982,7 +1125,7 @@
         <v>25.75</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>8</v>
@@ -1006,8 +1149,11 @@
         <f t="shared" si="2"/>
         <v>127.54545454545455</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="J8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>9</v>
@@ -1032,7 +1178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
         <v>10</v>
@@ -1057,7 +1203,7 @@
         <v>4.4444444444444446</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>11</v>
@@ -1082,7 +1228,7 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -1100,14 +1246,17 @@
         <v>30</v>
       </c>
       <c r="G12" s="2">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="J12" s="22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>13</v>
@@ -1132,7 +1281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>14</v>
@@ -1157,7 +1306,7 @@
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
         <v>45</v>
@@ -1186,7 +1335,7 @@
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
         <v>15</v>
@@ -1210,12 +1359,14 @@
         <f t="shared" si="2"/>
         <v>74.285714285714292</v>
       </c>
-      <c r="J16" s="9"/>
+      <c r="J16" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>16</v>
@@ -1239,12 +1390,14 @@
         <f t="shared" si="2"/>
         <v>250</v>
       </c>
-      <c r="J17" s="9"/>
+      <c r="J17" s="21" t="s">
+        <v>124</v>
+      </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="7" t="s">
         <v>17</v>
@@ -1270,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
         <v>18</v>
@@ -1295,7 +1448,7 @@
         <v>3.6111111111111112</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
         <v>46</v>
@@ -1320,7 +1473,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
@@ -1344,8 +1497,11 @@
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="J21" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -1370,7 +1526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
         <v>21</v>
@@ -1395,7 +1551,7 @@
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" t="s">
         <v>47</v>
@@ -1420,7 +1576,7 @@
         <v>35.333333333333336</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="2" t="s">
         <v>22</v>
@@ -1444,8 +1600,11 @@
         <f t="shared" si="2"/>
         <v>68.666666666666671</v>
       </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="J25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="2" t="s">
         <v>23</v>
@@ -1470,7 +1629,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="2" t="s">
         <v>24</v>
@@ -1495,7 +1654,7 @@
         <v>8.6206896551724146</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="2" t="s">
         <v>25</v>
@@ -1525,7 +1684,7 @@
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="2" t="s">
         <v>26</v>
@@ -1550,12 +1709,14 @@
         <f t="shared" si="2"/>
         <v>135.83333333333334</v>
       </c>
-      <c r="J29" s="9"/>
+      <c r="J29" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" t="s">
         <v>27</v>
@@ -1584,7 +1745,7 @@
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" t="s">
         <v>28</v>
@@ -1613,7 +1774,7 @@
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="5" t="s">
         <v>49</v>
@@ -1642,7 +1803,7 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="2" t="s">
         <v>48</v>
@@ -1666,8 +1827,11 @@
         <f t="shared" si="2"/>
         <v>81.75</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="2" t="s">
         <v>29</v>
@@ -1688,11 +1852,14 @@
         <v>55</v>
       </c>
       <c r="I34">
-        <f t="shared" ref="I34:I37" si="3">IFERROR(D34/E34,"---")</f>
+        <f t="shared" ref="I34:I35" si="3">IFERROR(D34/E34,"---")</f>
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="J34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="14" t="s">
         <v>30</v>
@@ -1717,235 +1884,247 @@
         <f t="shared" si="3"/>
         <v>275</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="3"/>
-      <c r="B36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="2">
-        <v>225</v>
-      </c>
-      <c r="D36" s="2">
-        <v>350</v>
-      </c>
-      <c r="E36" s="2">
-        <v>35</v>
-      </c>
-      <c r="F36" s="2">
-        <v>60</v>
-      </c>
-      <c r="G36" s="2">
-        <v>40</v>
-      </c>
-      <c r="I36">
+      <c r="J35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+      <c r="B36" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="20">
+        <v>180</v>
+      </c>
+      <c r="D36" s="20">
+        <v>100</v>
+      </c>
+      <c r="E36" s="20">
+        <v>25</v>
+      </c>
+      <c r="F36" s="20">
+        <v>50</v>
+      </c>
+      <c r="G36" s="20">
+        <v>45</v>
+      </c>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9">
         <f>IFERROR(D36/E36,"---")</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C37" s="2">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D37" s="2">
-        <v>650</v>
+        <v>300</v>
       </c>
       <c r="E37" s="2">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F37" s="2">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="G37" s="2">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="I37">
         <f>IFERROR(D37/E37,"---")</f>
-        <v>16.25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C38" s="2">
+        <v>160</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1100</v>
+      </c>
+      <c r="E38" s="2">
+        <v>35</v>
+      </c>
+      <c r="F38" s="2">
+        <v>50</v>
+      </c>
+      <c r="G38" s="2">
+        <v>50</v>
+      </c>
+      <c r="I38">
+        <f t="shared" ref="I38" si="4">IFERROR(D38/E38,"---")</f>
+        <v>31.428571428571427</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="2">
+        <v>90</v>
+      </c>
+      <c r="D39" s="2">
+        <v>3100</v>
+      </c>
+      <c r="E39" s="2">
+        <v>35</v>
+      </c>
+      <c r="F39" s="2">
+        <v>35</v>
+      </c>
+      <c r="G39" s="2">
+        <v>65</v>
+      </c>
+      <c r="I39">
+        <f t="shared" ref="I39" si="5">IFERROR(D39/E39,"---")</f>
+        <v>88.571428571428569</v>
+      </c>
+      <c r="J39" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="2">
         <v>200</v>
       </c>
-      <c r="D38" s="2">
-        <v>1350</v>
-      </c>
-      <c r="E38" s="2">
-        <v>45</v>
-      </c>
-      <c r="F38" s="2">
+      <c r="D40" s="2">
+        <v>18000</v>
+      </c>
+      <c r="E40" s="2">
+        <v>65</v>
+      </c>
+      <c r="F40" s="2">
         <v>55</v>
       </c>
-      <c r="G38" s="2">
-        <v>45</v>
-      </c>
-      <c r="I38">
-        <f>IFERROR(D38/E38,"---")</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="20">
-        <v>115</v>
-      </c>
-      <c r="D39" s="20">
-        <v>2950</v>
-      </c>
-      <c r="E39" s="20">
-        <v>45</v>
-      </c>
-      <c r="F39" s="20">
-        <v>40</v>
-      </c>
-      <c r="G39" s="20">
-        <v>60</v>
-      </c>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9">
-        <f>IFERROR(D39/E39,"---")</f>
-        <v>65.555555555555557</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="19"/>
-      <c r="B40" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="C40" s="20">
-        <v>180</v>
-      </c>
-      <c r="D40" s="20">
-        <v>100</v>
-      </c>
-      <c r="E40" s="20">
-        <v>25</v>
-      </c>
-      <c r="F40" s="20">
+      <c r="G40" s="2">
         <v>50</v>
       </c>
-      <c r="G40" s="20">
-        <v>45</v>
-      </c>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9">
+      <c r="I40">
         <f>IFERROR(D40/E40,"---")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>276.92307692307691</v>
+      </c>
+      <c r="J40" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C41" s="2">
-        <v>180</v>
+        <v>225</v>
       </c>
       <c r="D41" s="2">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="E41" s="2">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F41" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G41" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I41">
         <f>IFERROR(D41/E41,"---")</f>
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3"/>
       <c r="B42" s="2" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C42" s="2">
-        <v>160</v>
+        <v>225</v>
       </c>
       <c r="D42" s="2">
-        <v>1100</v>
+        <v>650</v>
       </c>
       <c r="E42" s="2">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F42" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="G42" s="2">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I42">
-        <f t="shared" ref="I42" si="4">IFERROR(D42/E42,"---")</f>
-        <v>31.428571428571427</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <f>IFERROR(D42/E42,"---")</f>
+        <v>16.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C43" s="2">
-        <v>90</v>
+        <v>200</v>
       </c>
       <c r="D43" s="2">
-        <v>3100</v>
+        <v>1350</v>
       </c>
       <c r="E43" s="2">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="F43" s="2">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="G43" s="2">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="I43">
-        <f t="shared" ref="I43" si="5">IFERROR(D43/E43,"---")</f>
-        <v>88.571428571428569</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44" s="3"/>
-      <c r="B44" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C44" s="2">
-        <v>200</v>
-      </c>
-      <c r="D44" s="2">
-        <v>18000</v>
-      </c>
-      <c r="E44" s="2">
-        <v>65</v>
-      </c>
-      <c r="F44" s="2">
-        <v>55</v>
-      </c>
-      <c r="G44" s="2">
-        <v>50</v>
-      </c>
-      <c r="I44">
+        <f>IFERROR(D43/E43,"---")</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" s="19"/>
+      <c r="B44" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="20">
+        <v>115</v>
+      </c>
+      <c r="D44" s="20">
+        <v>2950</v>
+      </c>
+      <c r="E44" s="20">
+        <v>45</v>
+      </c>
+      <c r="F44" s="20">
+        <v>40</v>
+      </c>
+      <c r="G44" s="20">
+        <v>60</v>
+      </c>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9">
         <f>IFERROR(D44/E44,"---")</f>
-        <v>276.92307692307691</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>65.555555555555557</v>
+      </c>
+      <c r="J44" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" t="s">
         <v>37</v>
@@ -1966,11 +2145,11 @@
         <v>30</v>
       </c>
       <c r="I45">
-        <f t="shared" ref="I40:I52" si="6">IFERROR(D45/E45,"---")</f>
+        <f t="shared" ref="I45:I52" si="6">IFERROR(D45/E45,"---")</f>
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" t="s">
         <v>38</v>
@@ -1995,7 +2174,7 @@
         <v>30.90909090909091</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" t="s">
         <v>39</v>
@@ -2021,16 +2200,16 @@
         <v>58.333333333333336</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="2" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="C48" s="2">
         <v>125</v>
       </c>
       <c r="D48" s="2">
-        <v>7000</v>
+        <v>6500</v>
       </c>
       <c r="E48" s="2">
         <v>60</v>
@@ -2043,10 +2222,13 @@
       </c>
       <c r="I48">
         <f t="shared" si="6"/>
-        <v>116.66666666666667</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>108.33333333333333</v>
+      </c>
+      <c r="J48" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" t="s">
         <v>40</v>
@@ -2070,8 +2252,11 @@
         <f t="shared" si="6"/>
         <v>131.25</v>
       </c>
-    </row>
-    <row r="50" spans="1:9">
+      <c r="J49" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" t="s">
         <v>41</v>
@@ -2095,8 +2280,11 @@
         <f t="shared" si="6"/>
         <v>300</v>
       </c>
-    </row>
-    <row r="51" spans="1:9">
+      <c r="J50" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" t="s">
         <v>42</v>
@@ -2120,39 +2308,73 @@
         <f t="shared" si="6"/>
         <v>92.307692307692307</v>
       </c>
-    </row>
-    <row r="52" spans="1:9">
+      <c r="J51" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
-      <c r="B52" s="2" t="s">
+      <c r="B52" t="s">
+        <v>135</v>
+      </c>
+      <c r="C52">
+        <v>350</v>
+      </c>
+      <c r="D52">
+        <v>10000</v>
+      </c>
+      <c r="E52">
+        <v>70</v>
+      </c>
+      <c r="F52">
+        <v>80</v>
+      </c>
+      <c r="G52">
+        <v>20</v>
+      </c>
+      <c r="I52">
+        <f t="shared" ref="I52" si="7">IFERROR(D52/E52,"---")</f>
+        <v>142.85714285714286</v>
+      </c>
+      <c r="J52" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C53" s="2">
         <v>350</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D53" s="2">
         <v>24000</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E53" s="2">
         <v>90</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F53" s="2">
         <v>80</v>
       </c>
-      <c r="G52" s="2">
+      <c r="G53" s="2">
         <v>20</v>
       </c>
-      <c r="I52">
-        <f t="shared" si="6"/>
+      <c r="I53">
+        <f>IFERROR(D53/E53,"---")</f>
         <v>266.66666666666669</v>
       </c>
+      <c r="J53" t="s">
+        <v>136</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:I52">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="I2:I53">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -2165,43 +2387,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>56</v>
-      </c>
       <c r="E1" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -2220,10 +2442,10 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -2233,10 +2455,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2246,10 +2468,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2268,10 +2490,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -2290,10 +2512,10 @@
         <v>312.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -2312,10 +2534,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8">
         <v>9</v>
@@ -2325,10 +2547,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -2338,10 +2560,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10">
         <v>11</v>
@@ -2360,10 +2582,10 @@
         <v>83.333333333333329</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -2382,10 +2604,10 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -2395,10 +2617,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -2408,10 +2630,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" s="14">
         <v>10</v>
@@ -2424,10 +2646,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C15">
         <v>18</v>
@@ -2446,10 +2668,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C16">
         <v>18</v>
@@ -2459,10 +2681,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17">
         <v>18</v>
@@ -2472,10 +2694,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C18">
         <v>22</v>
@@ -2494,10 +2716,10 @@
         <v>21.818181818181817</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19">
         <v>20</v>
@@ -2512,14 +2734,14 @@
         <v>50</v>
       </c>
       <c r="G19">
-        <f t="shared" si="0"/>
+        <f>IFERROR(D19/E19,"---")</f>
         <v>133.33333333333334</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" s="2">
         <v>20</v>
@@ -2532,10 +2754,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21">
         <v>15</v>
@@ -2554,10 +2776,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22">
         <v>15</v>
@@ -2567,10 +2789,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23">
         <v>15</v>
@@ -2580,10 +2802,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="2">
         <f>15*1.2</f>
@@ -2597,10 +2819,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25">
         <v>15</v>
@@ -2619,10 +2841,10 @@
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="16"/>
       <c r="B26" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" s="15">
         <f>18*1.5</f>
@@ -2642,10 +2864,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C27">
         <v>15</v>
@@ -2664,10 +2886,10 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28">
         <v>15</v>
@@ -2677,10 +2899,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C29">
         <v>15</v>
@@ -2690,10 +2912,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="2">
         <f>15*1.2</f>
@@ -2707,10 +2929,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C31">
         <v>27</v>
@@ -2729,10 +2951,10 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C32">
         <v>27</v>
@@ -2742,10 +2964,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C33">
         <v>27</v>
@@ -2755,10 +2977,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C34">
         <v>36</v>
@@ -2777,10 +2999,10 @@
         <v>94.117647058823536</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C35" s="2">
         <v>32</v>
@@ -2793,10 +3015,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C36">
         <v>40</v>
@@ -2815,10 +3037,10 @@
         <v>36.363636363636367</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C37" s="2">
         <v>40</v>
@@ -2831,10 +3053,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C38">
         <v>36</v>
@@ -2853,10 +3075,10 @@
         <v>363.63636363636363</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="17"/>
       <c r="B39" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C39" s="15">
         <v>36</v>
@@ -2875,10 +3097,10 @@
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C40">
         <v>12</v>
@@ -2897,10 +3119,10 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C41">
         <v>12</v>
@@ -2910,10 +3132,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C42">
         <v>12</v>
@@ -2923,10 +3145,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C43">
         <v>36</v>
@@ -2945,10 +3167,10 @@
         <v>0.34285714285714286</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C44">
         <v>36</v>
@@ -2958,10 +3180,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C45">
         <v>36</v>
@@ -2971,10 +3193,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C46">
         <v>43</v>
@@ -2993,10 +3215,10 @@
         <v>55.555555555555557</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C47" s="2">
         <v>30</v>
@@ -3015,10 +3237,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C48" s="2">
         <v>30</v>
@@ -3031,10 +3253,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C49" s="2">
         <f>30*0.9</f>
@@ -3048,10 +3270,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C50">
         <v>44</v>
@@ -3070,10 +3292,10 @@
         <v>8.3333333333333339</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C51" s="2">
         <f>30*1.2</f>
@@ -3087,10 +3309,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C52" s="2">
         <v>38</v>
@@ -3103,10 +3325,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C53">
         <v>27</v>
@@ -3122,10 +3344,10 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
       <c r="B54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C54">
         <v>27</v>
@@ -3135,10 +3357,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
       <c r="B55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C55">
         <v>27</v>
@@ -3148,10 +3370,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="11"/>
       <c r="B56" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C56" s="2">
         <v>32</v>
@@ -3164,10 +3386,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="B57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C57">
         <v>50</v>
@@ -3186,10 +3408,10 @@
         <v>208.33333333333334</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C58">
         <v>40</v>
@@ -3208,10 +3430,10 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C59">
         <v>25</v>
@@ -3230,10 +3452,10 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C60">
         <v>30</v>
@@ -3252,10 +3474,10 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="18"/>
       <c r="B61" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C61" s="15">
         <v>30</v>
@@ -3268,10 +3490,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
       <c r="B62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C62">
         <v>5</v>
@@ -3290,10 +3512,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="12"/>
       <c r="B63" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C63">
         <v>5</v>
@@ -3312,10 +3534,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="B64" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C64">
         <v>5</v>
@@ -3334,10 +3556,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C65">
         <v>20</v>
@@ -3360,9 +3582,565 @@
   <conditionalFormatting sqref="G2:G65">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>45</v>
+      </c>
+      <c r="H2" s="23">
+        <f>IFERROR(D2/E2,"---")</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>55</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>45</v>
+      </c>
+      <c r="H3" s="23">
+        <f t="shared" ref="H3:H21" si="0">IFERROR(D3/E3,"---")</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>505</v>
+      </c>
+      <c r="E4">
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <v>40</v>
+      </c>
+      <c r="H4" s="23">
+        <f t="shared" si="0"/>
+        <v>20.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="2">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
+        <v>250</v>
+      </c>
+      <c r="E5" s="2">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2">
+        <v>35</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H5" s="23">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="2">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2">
+        <v>900</v>
+      </c>
+      <c r="E6" s="2">
+        <v>35</v>
+      </c>
+      <c r="F6" s="2">
+        <v>30</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H6" s="23">
+        <f t="shared" si="0"/>
+        <v>25.714285714285715</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
+      </c>
+      <c r="H7" s="23">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>65</v>
+      </c>
+      <c r="E8">
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <v>50</v>
+      </c>
+      <c r="H8" s="23">
+        <f t="shared" si="0"/>
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C9">
+        <f>30*0.9</f>
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>515</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="F9">
+        <v>45</v>
+      </c>
+      <c r="H9" s="23">
+        <f t="shared" si="0"/>
+        <v>17.166666666666668</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>1515</v>
+      </c>
+      <c r="E10">
+        <v>30</v>
+      </c>
+      <c r="F10">
+        <v>25</v>
+      </c>
+      <c r="H10" s="23">
+        <f t="shared" si="0"/>
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11">
+        <f>30*1.2</f>
+        <v>36</v>
+      </c>
+      <c r="D11">
+        <v>4500</v>
+      </c>
+      <c r="E11">
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>55</v>
+      </c>
+      <c r="H11" s="23">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C12">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>20000</v>
+      </c>
+      <c r="E12">
+        <v>75</v>
+      </c>
+      <c r="F12">
+        <v>70</v>
+      </c>
+      <c r="H12" s="23">
+        <f t="shared" si="0"/>
+        <v>266.66666666666669</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C13" s="2">
+        <v>12</v>
+      </c>
+      <c r="D13" s="2">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2">
+        <v>15</v>
+      </c>
+      <c r="F13" s="2">
+        <v>20</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="23">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C14" s="2">
+        <v>12</v>
+      </c>
+      <c r="D14" s="2">
+        <v>70</v>
+      </c>
+      <c r="E14" s="2">
+        <v>20</v>
+      </c>
+      <c r="F14" s="2">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="23">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="2">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2">
+        <v>520</v>
+      </c>
+      <c r="E15" s="2">
+        <v>25</v>
+      </c>
+      <c r="F15" s="2">
+        <v>20</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="23">
+        <f t="shared" si="0"/>
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C16" s="2">
+        <v>40</v>
+      </c>
+      <c r="D16" s="2">
+        <v>50</v>
+      </c>
+      <c r="E16" s="2">
+        <v>40</v>
+      </c>
+      <c r="F16" s="2">
+        <v>60</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="23">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C17" s="2">
+        <v>40</v>
+      </c>
+      <c r="D17" s="2">
+        <v>150</v>
+      </c>
+      <c r="E17" s="2">
+        <v>45</v>
+      </c>
+      <c r="F17" s="2">
+        <v>60</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="23">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C18" s="2">
+        <f>40*0.9</f>
+        <v>36</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1050</v>
+      </c>
+      <c r="E18" s="2">
+        <v>50</v>
+      </c>
+      <c r="F18" s="2">
+        <v>55</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="23">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" s="2">
+        <v>35</v>
+      </c>
+      <c r="D19" s="2">
+        <v>180</v>
+      </c>
+      <c r="E19" s="2">
+        <v>25</v>
+      </c>
+      <c r="F19" s="2">
+        <v>50</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="23">
+        <f t="shared" si="0"/>
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" s="2">
+        <v>32</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1180</v>
+      </c>
+      <c r="E20" s="2">
+        <v>30</v>
+      </c>
+      <c r="F20" s="2">
+        <v>50</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="23">
+        <f t="shared" si="0"/>
+        <v>39.333333333333336</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" s="2">
+        <v>5</v>
+      </c>
+      <c r="D21" s="2">
+        <v>5000</v>
+      </c>
+      <c r="E21" s="2">
+        <v>50</v>
+      </c>
+      <c r="F21" s="2">
+        <v>10</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="23">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="H2:H21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>

</xml_diff>

<commit_message>
new armor mesh/textures, paker
</commit_message>
<xml_diff>
--- a/doc/items.xlsx
+++ b/doc/items.xlsx
@@ -1,24 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr codeName="Ten_skoroszyt"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomasz.zielski\Source\Repos\carpg\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="armor" sheetId="1" r:id="rId1"/>
     <sheet name="weapon" sheetId="2" r:id="rId2"/>
     <sheet name="shield" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="162">
   <si>
     <t>def</t>
   </si>
@@ -130,15 +125,6 @@
     <t>antimage</t>
   </si>
   <si>
-    <t>plated</t>
-  </si>
-  <si>
-    <t>plated hq</t>
-  </si>
-  <si>
-    <t>plated mith</t>
-  </si>
-  <si>
     <t>plate</t>
   </si>
   <si>
@@ -182,9 +168,6 @@
   </si>
   <si>
     <t>splint mith</t>
-  </si>
-  <si>
-    <t>plated m</t>
   </si>
   <si>
     <t>name</t>
@@ -529,8 +512,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -638,7 +621,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -651,10 +633,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -927,22 +910,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Arkusz1"/>
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
@@ -950,49 +933,49 @@
     <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="10" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H1" s="9"/>
+      <c r="I1" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
         <v>45</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="5">
         <v>5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="5">
         <v>5</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="5">
         <v>25</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="5">
         <v>90</v>
       </c>
       <c r="I2">
@@ -1000,24 +983,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>45</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="5">
         <v>55</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="5">
         <v>7</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="5">
         <v>25</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="5">
         <v>95</v>
       </c>
       <c r="I3">
@@ -1025,24 +1008,24 @@
         <v>7.8571428571428568</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="1"/>
-      <c r="B4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="5">
         <v>40</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="5">
         <v>505</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="5">
         <v>15</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="5">
         <v>25</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="5">
         <v>95</v>
       </c>
       <c r="I4">
@@ -1050,7 +1033,7 @@
         <v>33.666666666666664</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>5</v>
@@ -1075,7 +1058,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>6</v>
@@ -1100,7 +1083,7 @@
         <v>5.416666666666667</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>7</v>
@@ -1125,7 +1108,7 @@
         <v>25.75</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>8</v>
@@ -1150,10 +1133,10 @@
         <v>127.54545454545455</v>
       </c>
       <c r="J8" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>9</v>
@@ -1178,7 +1161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
         <v>10</v>
@@ -1203,7 +1186,7 @@
         <v>4.4444444444444446</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>11</v>
@@ -1228,7 +1211,7 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
@@ -1252,11 +1235,11 @@
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="J12" s="22" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J12" s="20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
         <v>13</v>
@@ -1281,7 +1264,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>14</v>
@@ -1306,10 +1289,10 @@
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15">
         <v>100</v>
@@ -1330,12 +1313,12 @@
         <f t="shared" si="2"/>
         <v>31.428571428571427</v>
       </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
         <v>15</v>
@@ -1359,14 +1342,14 @@
         <f t="shared" si="2"/>
         <v>74.285714285714292</v>
       </c>
-      <c r="J16" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J16" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>16</v>
@@ -1390,57 +1373,57 @@
         <f t="shared" si="2"/>
         <v>250</v>
       </c>
-      <c r="J17" s="21" t="s">
-        <v>124</v>
-      </c>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J17" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="6"/>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="22">
         <v>115</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="22">
         <v>15</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="22">
         <v>15</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="22">
         <v>40</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="22">
         <v>55</v>
       </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8">
+      <c r="H18" s="7"/>
+      <c r="I18" s="7">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" s="4"/>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="5">
         <v>115</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="5">
         <v>65</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="5">
         <v>18</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="5">
         <v>40</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="5">
         <v>60</v>
       </c>
       <c r="I19">
@@ -1448,24 +1431,24 @@
         <v>3.6111111111111112</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" s="4"/>
-      <c r="B20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="5">
         <v>100</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="5">
         <v>1100</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="5">
         <v>25</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="5">
         <v>40</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="5">
         <v>60</v>
       </c>
       <c r="I20">
@@ -1473,7 +1456,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
@@ -1497,11 +1480,11 @@
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
-      <c r="J21" s="22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J21" s="20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
         <v>20</v>
@@ -1526,7 +1509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
         <v>21</v>
@@ -1551,10 +1534,10 @@
         <v>6.666666666666667</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" s="4"/>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C24">
         <v>160</v>
@@ -1576,24 +1559,24 @@
         <v>35.333333333333336</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" s="4"/>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="5">
         <v>90</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="5">
         <v>2060</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="5">
         <v>30</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="5">
         <v>35</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="5">
         <v>65</v>
       </c>
       <c r="I25">
@@ -1601,27 +1584,27 @@
         <v>68.666666666666671</v>
       </c>
       <c r="J25" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="4"/>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="5">
         <v>150</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="5">
         <v>150</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="5">
         <v>25</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="5">
         <v>50</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="5">
         <v>55</v>
       </c>
       <c r="I26">
@@ -1629,24 +1612,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" s="4"/>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="5">
         <v>150</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="5">
         <v>250</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="5">
         <v>29</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="5">
         <v>50</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="5">
         <v>60</v>
       </c>
       <c r="I27">
@@ -1654,69 +1637,69 @@
         <v>8.6206896551724146</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" s="4"/>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="5">
         <f>150*0.9</f>
         <v>135</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="5">
         <v>1150</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="5">
         <v>35</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="5">
         <v>45</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="5">
         <v>60</v>
       </c>
       <c r="I28">
         <f t="shared" si="2"/>
         <v>32.857142857142854</v>
       </c>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="4"/>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="5">
         <f>150*1.1</f>
         <v>165</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="5">
         <v>8150</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="5">
         <v>60</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="5">
         <v>50</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="5">
         <v>50</v>
       </c>
       <c r="I29">
         <f t="shared" si="2"/>
         <v>135.83333333333334</v>
       </c>
-      <c r="J29" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J29" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="4"/>
       <c r="B30" t="s">
         <v>27</v>
@@ -1740,12 +1723,12 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="4"/>
       <c r="B31" t="s">
         <v>28</v>
@@ -1769,15 +1752,15 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="4"/>
       <c r="B32" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C32">
         <v>120</v>
@@ -1798,29 +1781,29 @@
         <f t="shared" si="2"/>
         <v>31.75</v>
       </c>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" s="4"/>
-      <c r="B33" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="2">
+      <c r="B33" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="5">
         <v>65</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="5">
         <v>3270</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="5">
         <v>40</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="5">
         <v>30</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="5">
         <v>75</v>
       </c>
       <c r="I33">
@@ -1828,27 +1811,27 @@
         <v>81.75</v>
       </c>
       <c r="J33" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" s="4"/>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="5">
         <v>160</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="5">
         <v>6270</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="5">
         <v>55</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="5">
         <v>50</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="5">
         <v>55</v>
       </c>
       <c r="I34">
@@ -1856,143 +1839,143 @@
         <v>114</v>
       </c>
       <c r="J34" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="15"/>
+      <c r="B35" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="14">
+      <c r="C35" s="13">
         <v>135</v>
       </c>
-      <c r="D35" s="14">
+      <c r="D35" s="13">
         <v>22000</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="13">
         <v>80</v>
       </c>
-      <c r="F35" s="14">
+      <c r="F35" s="13">
         <v>45</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="13">
         <v>65</v>
       </c>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15">
+      <c r="H35" s="14"/>
+      <c r="I35" s="14">
         <f t="shared" si="3"/>
         <v>275</v>
       </c>
       <c r="J35" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="18"/>
+      <c r="B36" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="20">
+      <c r="C36" s="23">
         <v>180</v>
       </c>
-      <c r="D36" s="20">
-        <v>100</v>
-      </c>
-      <c r="E36" s="20">
-        <v>25</v>
-      </c>
-      <c r="F36" s="20">
+      <c r="D36" s="23">
+        <v>200</v>
+      </c>
+      <c r="E36" s="23">
+        <v>30</v>
+      </c>
+      <c r="F36" s="23">
         <v>50</v>
       </c>
-      <c r="G36" s="20">
+      <c r="G36" s="23">
         <v>45</v>
       </c>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9">
+      <c r="H36" s="8"/>
+      <c r="I36" s="8">
         <f>IFERROR(D36/E36,"---")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" s="3"/>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="5">
         <v>180</v>
       </c>
-      <c r="D37" s="2">
-        <v>300</v>
-      </c>
-      <c r="E37" s="2">
-        <v>30</v>
-      </c>
-      <c r="F37" s="2">
+      <c r="D37" s="5">
+        <v>400</v>
+      </c>
+      <c r="E37" s="5">
+        <v>35</v>
+      </c>
+      <c r="F37" s="5">
         <v>50</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37" s="5">
         <v>50</v>
       </c>
       <c r="I37">
         <f>IFERROR(D37/E37,"---")</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+        <v>11.428571428571429</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" s="3"/>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="5">
+        <v>160</v>
+      </c>
+      <c r="D38" s="5">
+        <v>1200</v>
+      </c>
+      <c r="E38" s="5">
+        <v>40</v>
+      </c>
+      <c r="F38" s="5">
         <v>50</v>
       </c>
-      <c r="C38" s="2">
-        <v>160</v>
-      </c>
-      <c r="D38" s="2">
-        <v>1100</v>
-      </c>
-      <c r="E38" s="2">
-        <v>35</v>
-      </c>
-      <c r="F38" s="2">
-        <v>50</v>
-      </c>
-      <c r="G38" s="2">
+      <c r="G38" s="5">
         <v>50</v>
       </c>
       <c r="I38">
         <f t="shared" ref="I38" si="4">IFERROR(D38/E38,"---")</f>
-        <v>31.428571428571427</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" s="3"/>
-      <c r="B39" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C39" s="2">
+      <c r="B39" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="5">
         <v>90</v>
       </c>
-      <c r="D39" s="2">
-        <v>3100</v>
-      </c>
-      <c r="E39" s="2">
+      <c r="D39" s="5">
+        <v>3200</v>
+      </c>
+      <c r="E39" s="5">
+        <v>40</v>
+      </c>
+      <c r="F39" s="5">
         <v>35</v>
       </c>
-      <c r="F39" s="2">
-        <v>35</v>
-      </c>
-      <c r="G39" s="2">
+      <c r="G39" s="5">
         <v>65</v>
       </c>
       <c r="I39">
         <f t="shared" ref="I39" si="5">IFERROR(D39/E39,"---")</f>
-        <v>88.571428571428569</v>
+        <v>80</v>
       </c>
       <c r="J39" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="3"/>
       <c r="B40" s="2" t="s">
         <v>33</v>
@@ -2004,7 +1987,7 @@
         <v>18000</v>
       </c>
       <c r="E40" s="2">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F40" s="2">
         <v>55</v>
@@ -2014,367 +1997,263 @@
       </c>
       <c r="I40">
         <f>IFERROR(D40/E40,"---")</f>
-        <v>276.92307692307691</v>
+        <v>257.14285714285717</v>
       </c>
       <c r="J40" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="3"/>
-      <c r="B41" s="2" t="s">
+      <c r="B41" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41">
+        <v>250</v>
+      </c>
+      <c r="D41">
+        <v>1500</v>
+      </c>
+      <c r="E41">
+        <v>50</v>
+      </c>
+      <c r="F41">
+        <v>70</v>
+      </c>
+      <c r="G41">
+        <v>30</v>
+      </c>
+      <c r="I41">
+        <f t="shared" ref="I41:I47" si="6">IFERROR(D41/E41,"---")</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="3"/>
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C42">
+        <v>250</v>
+      </c>
+      <c r="D42">
+        <v>1700</v>
+      </c>
+      <c r="E42">
+        <v>55</v>
+      </c>
+      <c r="F42">
+        <v>70</v>
+      </c>
+      <c r="G42">
+        <v>35</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="6"/>
+        <v>30.90909090909091</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="3"/>
+      <c r="B43" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43">
+        <f>250*0.9</f>
         <v>225</v>
       </c>
-      <c r="D41" s="2">
-        <v>350</v>
-      </c>
-      <c r="E41" s="2">
+      <c r="D43">
+        <v>3500</v>
+      </c>
+      <c r="E43" s="5">
+        <v>60</v>
+      </c>
+      <c r="F43">
+        <v>65</v>
+      </c>
+      <c r="G43">
         <v>35</v>
       </c>
-      <c r="F41" s="2">
+      <c r="I43">
+        <f t="shared" si="6"/>
+        <v>58.333333333333336</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="3"/>
+      <c r="B44" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" s="5">
+        <v>125</v>
+      </c>
+      <c r="D44" s="5">
+        <v>6500</v>
+      </c>
+      <c r="E44" s="5">
         <v>60</v>
       </c>
-      <c r="G41" s="2">
+      <c r="F44" s="5">
         <v>40</v>
       </c>
-      <c r="I41">
-        <f>IFERROR(D41/E41,"---")</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42" s="2">
-        <v>225</v>
-      </c>
-      <c r="D42" s="2">
-        <v>650</v>
-      </c>
-      <c r="E42" s="2">
-        <v>40</v>
-      </c>
-      <c r="F42" s="2">
-        <v>60</v>
-      </c>
-      <c r="G42" s="2">
-        <v>45</v>
-      </c>
-      <c r="I42">
-        <f>IFERROR(D42/E42,"---")</f>
-        <v>16.25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-      <c r="B43" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="2">
-        <v>200</v>
-      </c>
-      <c r="D43" s="2">
-        <v>1350</v>
-      </c>
-      <c r="E43" s="2">
-        <v>45</v>
-      </c>
-      <c r="F43" s="2">
+      <c r="G44" s="5">
         <v>55</v>
       </c>
-      <c r="G43" s="2">
-        <v>45</v>
-      </c>
-      <c r="I43">
-        <f>IFERROR(D43/E43,"---")</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="B44" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="C44" s="20">
-        <v>115</v>
-      </c>
-      <c r="D44" s="20">
-        <v>2950</v>
-      </c>
-      <c r="E44" s="20">
-        <v>45</v>
-      </c>
-      <c r="F44" s="20">
-        <v>40</v>
-      </c>
-      <c r="G44" s="20">
-        <v>60</v>
-      </c>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9">
-        <f>IFERROR(D44/E44,"---")</f>
-        <v>65.555555555555557</v>
+      <c r="I44">
+        <f t="shared" si="6"/>
+        <v>108.33333333333333</v>
       </c>
       <c r="J44" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="3"/>
       <c r="B45" t="s">
         <v>37</v>
       </c>
       <c r="C45">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="D45">
-        <v>1500</v>
+        <v>10500</v>
       </c>
       <c r="E45">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F45">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G45">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="I45">
-        <f t="shared" ref="I45:I52" si="6">IFERROR(D45/E45,"---")</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v>131.25</v>
+      </c>
+      <c r="J45" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" s="3"/>
       <c r="B46" t="s">
         <v>38</v>
       </c>
       <c r="C46">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="D46">
-        <v>1700</v>
+        <v>30000</v>
       </c>
       <c r="E46">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="F46">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G46">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I46">
         <f t="shared" si="6"/>
-        <v>30.90909090909091</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="J46" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" s="3"/>
       <c r="B47" t="s">
         <v>39</v>
       </c>
       <c r="C47">
-        <f>250*0.9</f>
-        <v>225</v>
+        <v>350</v>
       </c>
       <c r="D47">
-        <v>3500</v>
-      </c>
-      <c r="E47" s="5">
-        <v>60</v>
+        <v>6000</v>
+      </c>
+      <c r="E47">
+        <v>65</v>
       </c>
       <c r="F47">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="G47">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="I47">
         <f t="shared" si="6"/>
-        <v>58.333333333333336</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+        <v>92.307692307692307</v>
+      </c>
+      <c r="J47" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" s="3"/>
-      <c r="B48" s="2" t="s">
+      <c r="B48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48">
+        <v>350</v>
+      </c>
+      <c r="D48">
+        <v>10000</v>
+      </c>
+      <c r="E48">
+        <v>70</v>
+      </c>
+      <c r="F48">
+        <v>80</v>
+      </c>
+      <c r="G48">
+        <v>20</v>
+      </c>
+      <c r="I48">
+        <f t="shared" ref="I48" si="7">IFERROR(D48/E48,"---")</f>
+        <v>142.85714285714286</v>
+      </c>
+      <c r="J48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="3"/>
+      <c r="B49" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="2">
+        <v>350</v>
+      </c>
+      <c r="D49" s="2">
+        <v>24000</v>
+      </c>
+      <c r="E49" s="2">
+        <v>90</v>
+      </c>
+      <c r="F49" s="2">
+        <v>80</v>
+      </c>
+      <c r="G49" s="2">
+        <v>20</v>
+      </c>
+      <c r="I49">
+        <f>IFERROR(D49/E49,"---")</f>
+        <v>266.66666666666669</v>
+      </c>
+      <c r="J49" t="s">
         <v>132</v>
       </c>
-      <c r="C48" s="2">
-        <v>125</v>
-      </c>
-      <c r="D48" s="2">
-        <v>6500</v>
-      </c>
-      <c r="E48" s="2">
-        <v>60</v>
-      </c>
-      <c r="F48" s="2">
-        <v>40</v>
-      </c>
-      <c r="G48" s="2">
-        <v>55</v>
-      </c>
-      <c r="I48">
-        <f t="shared" si="6"/>
-        <v>108.33333333333333</v>
-      </c>
-      <c r="J48" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" t="s">
-        <v>40</v>
-      </c>
-      <c r="C49">
-        <v>300</v>
-      </c>
-      <c r="D49">
-        <v>10500</v>
-      </c>
-      <c r="E49">
-        <v>80</v>
-      </c>
-      <c r="F49">
-        <v>75</v>
-      </c>
-      <c r="G49">
-        <v>25</v>
-      </c>
-      <c r="I49">
-        <f t="shared" si="6"/>
-        <v>131.25</v>
-      </c>
-      <c r="J49" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" t="s">
-        <v>41</v>
-      </c>
-      <c r="C50">
-        <v>300</v>
-      </c>
-      <c r="D50">
-        <v>30000</v>
-      </c>
-      <c r="E50">
-        <v>100</v>
-      </c>
-      <c r="F50">
-        <v>75</v>
-      </c>
-      <c r="G50">
-        <v>25</v>
-      </c>
-      <c r="I50">
-        <f t="shared" si="6"/>
-        <v>300</v>
-      </c>
-      <c r="J50" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" t="s">
-        <v>42</v>
-      </c>
-      <c r="C51">
-        <v>350</v>
-      </c>
-      <c r="D51">
-        <v>6000</v>
-      </c>
-      <c r="E51">
-        <v>65</v>
-      </c>
-      <c r="F51">
-        <v>80</v>
-      </c>
-      <c r="G51">
-        <v>20</v>
-      </c>
-      <c r="I51">
-        <f t="shared" si="6"/>
-        <v>92.307692307692307</v>
-      </c>
-      <c r="J51" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" t="s">
-        <v>135</v>
-      </c>
-      <c r="C52">
-        <v>350</v>
-      </c>
-      <c r="D52">
-        <v>10000</v>
-      </c>
-      <c r="E52">
-        <v>70</v>
-      </c>
-      <c r="F52">
-        <v>80</v>
-      </c>
-      <c r="G52">
-        <v>20</v>
-      </c>
-      <c r="I52">
-        <f t="shared" ref="I52" si="7">IFERROR(D52/E52,"---")</f>
-        <v>142.85714285714286</v>
-      </c>
-      <c r="J52" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-      <c r="B53" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C53" s="2">
-        <v>350</v>
-      </c>
-      <c r="D53" s="2">
-        <v>24000</v>
-      </c>
-      <c r="E53" s="2">
-        <v>90</v>
-      </c>
-      <c r="F53" s="2">
-        <v>80</v>
-      </c>
-      <c r="G53" s="2">
-        <v>20</v>
-      </c>
-      <c r="I53">
-        <f>IFERROR(D53/E53,"---")</f>
-        <v>266.66666666666669</v>
-      </c>
-      <c r="J53" t="s">
-        <v>136</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I2:I53">
+  <conditionalFormatting sqref="I2:I49">
     <cfRule type="colorScale" priority="4">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -2387,43 +2266,43 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:7">
+      <c r="B1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -2442,10 +2321,10 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -2455,10 +2334,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2468,10 +2347,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -2490,10 +2369,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -2512,10 +2391,10 @@
         <v>312.5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -2534,10 +2413,10 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C8">
         <v>9</v>
@@ -2547,10 +2426,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C9">
         <v>9</v>
@@ -2560,10 +2439,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C10">
         <v>11</v>
@@ -2582,10 +2461,10 @@
         <v>83.333333333333329</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -2604,10 +2483,10 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C12">
         <v>10</v>
@@ -2617,10 +2496,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="1"/>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C13">
         <v>10</v>
@@ -2630,26 +2509,26 @@
         <v>---</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="14">
+    <row r="14" spans="1:7">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="13">
         <v>10</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
       <c r="G14" t="str">
         <f t="shared" si="0"/>
         <v>---</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C15">
         <v>18</v>
@@ -2668,10 +2547,10 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="4"/>
       <c r="B16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C16">
         <v>18</v>
@@ -2681,10 +2560,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C17">
         <v>18</v>
@@ -2694,10 +2573,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
       <c r="A18" s="4"/>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C18">
         <v>22</v>
@@ -2716,10 +2595,10 @@
         <v>21.818181818181817</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C19">
         <v>20</v>
@@ -2738,10 +2617,10 @@
         <v>133.33333333333334</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C20" s="2">
         <v>20</v>
@@ -2754,10 +2633,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C21">
         <v>15</v>
@@ -2776,10 +2655,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C22">
         <v>15</v>
@@ -2789,10 +2668,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C23">
         <v>15</v>
@@ -2802,10 +2681,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7">
       <c r="A24" s="4"/>
       <c r="B24" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C24" s="2">
         <f>15*1.2</f>
@@ -2819,10 +2698,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7">
       <c r="A25" s="4"/>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C25">
         <v>15</v>
@@ -2841,22 +2720,22 @@
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="15">
+    <row r="26" spans="1:7">
+      <c r="A26" s="15"/>
+      <c r="B26" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="14">
         <f>18*1.5</f>
         <v>27</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="14">
         <v>25</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="14">
         <v>40</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="14">
         <v>55</v>
       </c>
       <c r="G26">
@@ -2864,10 +2743,10 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7">
       <c r="A27" s="3"/>
       <c r="B27" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C27">
         <v>15</v>
@@ -2886,10 +2765,10 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7">
       <c r="A28" s="3"/>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C28">
         <v>15</v>
@@ -2899,10 +2778,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7">
       <c r="A29" s="3"/>
       <c r="B29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C29">
         <v>15</v>
@@ -2912,10 +2791,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7">
       <c r="A30" s="3"/>
       <c r="B30" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C30" s="2">
         <f>15*1.2</f>
@@ -2929,10 +2808,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7">
       <c r="A31" s="3"/>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C31">
         <v>27</v>
@@ -2951,10 +2830,10 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7">
       <c r="A32" s="3"/>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C32">
         <v>27</v>
@@ -2964,10 +2843,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7">
       <c r="A33" s="3"/>
       <c r="B33" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C33">
         <v>27</v>
@@ -2977,10 +2856,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34" s="3"/>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C34">
         <v>36</v>
@@ -2999,10 +2878,10 @@
         <v>94.117647058823536</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35" s="3"/>
       <c r="B35" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C35" s="2">
         <v>32</v>
@@ -3015,10 +2894,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36" s="3"/>
       <c r="B36" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C36">
         <v>40</v>
@@ -3037,10 +2916,10 @@
         <v>36.363636363636367</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7">
       <c r="A37" s="3"/>
       <c r="B37" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C37" s="2">
         <v>40</v>
@@ -3053,10 +2932,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7">
       <c r="A38" s="3"/>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C38">
         <v>36</v>
@@ -3075,21 +2954,21 @@
         <v>363.63636363636363</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
-      <c r="B39" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C39" s="15">
+    <row r="39" spans="1:7">
+      <c r="A39" s="16"/>
+      <c r="B39" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="14">
         <v>36</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="14">
         <v>25</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="14">
         <v>35</v>
       </c>
-      <c r="F39" s="15">
+      <c r="F39" s="14">
         <v>75</v>
       </c>
       <c r="G39">
@@ -3097,10 +2976,10 @@
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
+    <row r="40" spans="1:7">
+      <c r="A40" s="10"/>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C40">
         <v>12</v>
@@ -3119,10 +2998,10 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
+    <row r="41" spans="1:7">
+      <c r="A41" s="10"/>
       <c r="B41" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C41">
         <v>12</v>
@@ -3132,10 +3011,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
+    <row r="42" spans="1:7">
+      <c r="A42" s="10"/>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C42">
         <v>12</v>
@@ -3145,10 +3024,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
+    <row r="43" spans="1:7">
+      <c r="A43" s="10"/>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C43">
         <v>36</v>
@@ -3167,10 +3046,10 @@
         <v>0.34285714285714286</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
+    <row r="44" spans="1:7">
+      <c r="A44" s="10"/>
       <c r="B44" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C44">
         <v>36</v>
@@ -3180,10 +3059,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="11"/>
+    <row r="45" spans="1:7">
+      <c r="A45" s="10"/>
       <c r="B45" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C45">
         <v>36</v>
@@ -3193,10 +3072,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
+    <row r="46" spans="1:7">
+      <c r="A46" s="10"/>
       <c r="B46" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C46">
         <v>43</v>
@@ -3215,10 +3094,10 @@
         <v>55.555555555555557</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
+    <row r="47" spans="1:7">
+      <c r="A47" s="10"/>
       <c r="B47" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C47" s="2">
         <v>30</v>
@@ -3237,10 +3116,10 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
+    <row r="48" spans="1:7">
+      <c r="A48" s="10"/>
       <c r="B48" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C48" s="2">
         <v>30</v>
@@ -3253,10 +3132,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
+    <row r="49" spans="1:7">
+      <c r="A49" s="10"/>
       <c r="B49" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C49" s="2">
         <f>30*0.9</f>
@@ -3270,10 +3149,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
+    <row r="50" spans="1:7">
+      <c r="A50" s="10"/>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C50">
         <v>44</v>
@@ -3292,10 +3171,10 @@
         <v>8.3333333333333339</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="11"/>
+    <row r="51" spans="1:7">
+      <c r="A51" s="10"/>
       <c r="B51" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C51" s="2">
         <f>30*1.2</f>
@@ -3309,10 +3188,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
+    <row r="52" spans="1:7">
+      <c r="A52" s="10"/>
       <c r="B52" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C52" s="2">
         <v>38</v>
@@ -3325,10 +3204,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="11"/>
+    <row r="53" spans="1:7">
+      <c r="A53" s="10"/>
       <c r="B53" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C53">
         <v>27</v>
@@ -3344,10 +3223,10 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
+    <row r="54" spans="1:7">
+      <c r="A54" s="10"/>
       <c r="B54" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C54">
         <v>27</v>
@@ -3357,10 +3236,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
+    <row r="55" spans="1:7">
+      <c r="A55" s="10"/>
       <c r="B55" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C55">
         <v>27</v>
@@ -3370,10 +3249,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="11"/>
+    <row r="56" spans="1:7">
+      <c r="A56" s="10"/>
       <c r="B56" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C56" s="2">
         <v>32</v>
@@ -3386,10 +3265,10 @@
         <v>---</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="11"/>
+    <row r="57" spans="1:7">
+      <c r="A57" s="10"/>
       <c r="B57" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C57">
         <v>50</v>
@@ -3408,10 +3287,10 @@
         <v>208.33333333333334</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="11"/>
+    <row r="58" spans="1:7">
+      <c r="A58" s="10"/>
       <c r="B58" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C58">
         <v>40</v>
@@ -3430,10 +3309,10 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="11"/>
+    <row r="59" spans="1:7">
+      <c r="A59" s="10"/>
       <c r="B59" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C59">
         <v>25</v>
@@ -3452,10 +3331,10 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="11"/>
+    <row r="60" spans="1:7">
+      <c r="A60" s="10"/>
       <c r="B60" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C60">
         <v>30</v>
@@ -3474,26 +3353,26 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="18"/>
-      <c r="B61" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="C61" s="15">
+    <row r="61" spans="1:7">
+      <c r="A61" s="17"/>
+      <c r="B61" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="C61" s="14">
         <v>30</v>
       </c>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
       <c r="G61" t="str">
         <f t="shared" si="0"/>
         <v>---</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="12"/>
+    <row r="62" spans="1:7">
+      <c r="A62" s="11"/>
       <c r="B62" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C62">
         <v>5</v>
@@ -3512,10 +3391,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="12"/>
+    <row r="63" spans="1:7">
+      <c r="A63" s="11"/>
       <c r="B63" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C63">
         <v>5</v>
@@ -3534,10 +3413,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
+    <row r="64" spans="1:7">
+      <c r="A64" s="11"/>
       <c r="B64" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C64">
         <v>5</v>
@@ -3556,10 +3435,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
+    <row r="65" spans="1:7">
+      <c r="A65" s="11"/>
       <c r="B65" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C65">
         <v>20</v>
@@ -3582,9 +3461,9 @@
   <conditionalFormatting sqref="G2:G65">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>
@@ -3597,31 +3476,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -3630,18 +3509,18 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C2">
         <v>25</v>
@@ -3655,17 +3534,17 @@
       <c r="F2">
         <v>45</v>
       </c>
-      <c r="H2" s="23">
+      <c r="H2" s="21">
         <f>IFERROR(D2/E2,"---")</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>25</v>
@@ -3679,17 +3558,17 @@
       <c r="F3">
         <v>45</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="21">
         <f t="shared" ref="H3:H21" si="0">IFERROR(D3/E3,"---")</f>
         <v>2.75</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C4">
         <v>23</v>
@@ -3703,17 +3582,17 @@
       <c r="F4">
         <v>40</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="21">
         <f t="shared" si="0"/>
         <v>20.2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C5" s="2">
         <v>20</v>
@@ -3728,19 +3607,19 @@
         <v>35</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="H5" s="23">
+        <v>161</v>
+      </c>
+      <c r="H5" s="21">
         <f t="shared" si="0"/>
         <v>8.3333333333333339</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C6" s="2">
         <v>19</v>
@@ -3755,19 +3634,19 @@
         <v>30</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="H6" s="23">
+        <v>161</v>
+      </c>
+      <c r="H6" s="21">
         <f t="shared" si="0"/>
         <v>25.714285714285715</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C7">
         <v>30</v>
@@ -3781,17 +3660,17 @@
       <c r="F7">
         <v>50</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="21">
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C8">
         <v>30</v>
@@ -3805,17 +3684,17 @@
       <c r="F8">
         <v>50</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="21">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C9">
         <f>30*0.9</f>
@@ -3830,17 +3709,17 @@
       <c r="F9">
         <v>45</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="21">
         <f t="shared" si="0"/>
         <v>17.166666666666668</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C10">
         <v>15</v>
@@ -3854,17 +3733,17 @@
       <c r="F10">
         <v>25</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="21">
         <f t="shared" si="0"/>
         <v>50.5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C11">
         <f>30*1.2</f>
@@ -3879,17 +3758,17 @@
       <c r="F11">
         <v>55</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="21">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C12">
         <v>50</v>
@@ -3903,17 +3782,17 @@
       <c r="F12">
         <v>70</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="21">
         <f t="shared" si="0"/>
         <v>266.66666666666669</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C13" s="2">
         <v>12</v>
@@ -3928,17 +3807,17 @@
         <v>20</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="23">
+      <c r="H13" s="21">
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C14" s="2">
         <v>12</v>
@@ -3953,17 +3832,17 @@
         <v>20</v>
       </c>
       <c r="G14" s="2"/>
-      <c r="H14" s="23">
+      <c r="H14" s="21">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C15" s="2">
         <v>11</v>
@@ -3978,17 +3857,17 @@
         <v>20</v>
       </c>
       <c r="G15" s="2"/>
-      <c r="H15" s="23">
+      <c r="H15" s="21">
         <f t="shared" si="0"/>
         <v>20.8</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C16" s="2">
         <v>40</v>
@@ -4003,17 +3882,17 @@
         <v>60</v>
       </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="23">
+      <c r="H16" s="21">
         <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C17" s="2">
         <v>40</v>
@@ -4028,17 +3907,17 @@
         <v>60</v>
       </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="23">
+      <c r="H17" s="21">
         <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C18" s="2">
         <f>40*0.9</f>
@@ -4054,17 +3933,17 @@
         <v>55</v>
       </c>
       <c r="G18" s="2"/>
-      <c r="H18" s="23">
+      <c r="H18" s="21">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C19" s="2">
         <v>35</v>
@@ -4079,17 +3958,17 @@
         <v>50</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="23">
+      <c r="H19" s="21">
         <f t="shared" si="0"/>
         <v>7.2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C20" s="2">
         <v>32</v>
@@ -4104,17 +3983,17 @@
         <v>50</v>
       </c>
       <c r="G20" s="2"/>
-      <c r="H20" s="23">
+      <c r="H20" s="21">
         <f t="shared" si="0"/>
         <v>39.333333333333336</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C21" s="2">
         <v>5</v>
@@ -4129,7 +4008,7 @@
         <v>10</v>
       </c>
       <c r="G21" s="2"/>
-      <c r="H21" s="23">
+      <c r="H21" s="21">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -4138,9 +4017,9 @@
   <conditionalFormatting sqref="H2:H21">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
+        <cfvo type="min" val="0"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="max" val="0"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>

</xml_diff>